<commit_message>
Update; some folder structure changes :/
</commit_message>
<xml_diff>
--- a/Other/tools.xlsx
+++ b/Other/tools.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uporto-my.sharepoint.com/personal/up202500848_up_pt/Documents/madsad2025_public/Other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="11_AD4DF034E34935FBC521DC34CF5A43225ADEDD8B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2B2A9DD-0B0B-49A8-AF51-90CD19AD81D5}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="11_AD4DF034E34935FBC521DC34CF5A43225ADEDD8B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8A5A06D-06BE-4810-8822-3CF5002CE723}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>Description</t>
   </si>
@@ -88,6 +88,21 @@
   </si>
   <si>
     <t>https://cran.r-project.org</t>
+  </si>
+  <si>
+    <t>ECD-I</t>
+  </si>
+  <si>
+    <t>https://www.knime.com/</t>
+  </si>
+  <si>
+    <t>Knime</t>
+  </si>
+  <si>
+    <t>Weka</t>
+  </si>
+  <si>
+    <t>http://www.cs.waikato.ac.nz/ml/weka/</t>
   </si>
 </sst>
 </file>
@@ -454,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -565,6 +580,34 @@
         <v>20</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{536B6582-5302-4F21-A87E-23CF6B707AC9}"/>
@@ -573,11 +616,13 @@
     <hyperlink ref="D5" r:id="rId4" xr:uid="{7EB07912-31F5-4A56-933D-80A75A5D481B}"/>
     <hyperlink ref="D6" r:id="rId5" xr:uid="{4053E495-25C0-4D6B-B0B7-2142D20F4401}"/>
     <hyperlink ref="D7" r:id="rId6" xr:uid="{508EBAE1-5D95-415C-81E2-8C5737E133CA}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{DC4B9827-FFDC-4370-9EB0-83A4C39B424F}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{15852FAF-9C3D-4CC3-897E-4E5686AF5C84}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
-    <tablePart r:id="rId7"/>
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>